<commit_message>
add some tcr test data
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1862CBC-274B-1544-B66F-0C2A459C9560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -34,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -140,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -210,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="72">
   <si>
     <t>LEGEND</t>
   </si>
@@ -405,25 +411,40 @@
   </si>
   <si>
     <t>#d</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.1.1.fastq.gz,/local/path/to/fwd.1.1.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.1.fastq.gz,/local/path/to/fwd.1.2.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP700.00</t>
+  </si>
+  <si>
+    <t>CTTTPP701.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -433,8 +454,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +497,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5FA3F0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2D2F6"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -504,20 +544,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,6 +570,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -571,7 +624,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,9 +656,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,6 +708,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -812,1117 +901,1176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="C4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="C5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="2" t="s">
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11">
+        <v>600</v>
+      </c>
+      <c r="F11">
+        <v>0.7</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12">
+        <v>650</v>
+      </c>
+      <c r="F12">
+        <v>0.8</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>64</v>
       </c>
@@ -1933,20 +2081,20 @@
     <mergeCell ref="B9:I9"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
-      <formula1>'Data Dictionary'!$B$2:$B$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{1AE57A24-A028-7D4A-BB26-668046DD637A}">
+      <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
-      <formula1>'Data Dictionary'!$C$2:$C$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6AAB7385-2BF3-3D4D-BD17-A1D472F06822}">
+      <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
-      <formula1>'Data Dictionary'!$D$2:$D$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{C25C07AA-5990-4044-B22D-C83425617F94}">
+      <formula1>"Agilent,Twist,IDT,NEB,Illumina - TruSeq Stranded PolyA mRNA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
-      <formula1>'Data Dictionary'!$E$2:$E$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{8502C027-0D19-4842-866A-42E86D371659}">
+      <formula1>"PolyA capture,Transcriptome capture,Ribo minus"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
-      <formula1>'Data Dictionary'!$F$2:$F$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{BD904793-8D16-0E4B-979F-874BF3736128}">
+      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1955,28 +2103,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -1986,8 +2134,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -2000,8 +2148,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
@@ -2014,8 +2162,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
@@ -2028,8 +2176,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
@@ -2042,8 +2190,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
@@ -2056,13 +2204,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
@@ -2075,8 +2223,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
@@ -2086,8 +2234,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
@@ -2097,8 +2245,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
@@ -2108,8 +2256,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C14" t="s">
@@ -2119,8 +2267,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
@@ -2130,8 +2278,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C16" t="s">
@@ -2141,8 +2289,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C17" t="s">
@@ -2159,34 +2307,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -2203,7 +2351,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>41</v>
       </c>
@@ -2220,7 +2368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -2234,7 +2382,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -2245,7 +2393,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
add tcr assay data generator
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1862CBC-274B-1544-B66F-0C2A459C9560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2B8F05-2EB1-6749-94C3-9445F585327E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,10 +428,10 @@
     <t>/local/path/to/rev.1.2.1.fastq.gz</t>
   </si>
   <si>
-    <t>CTTTPP700.00</t>
-  </si>
-  <si>
-    <t>CTTTPP701.00</t>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
   </si>
 </sst>
 </file>
@@ -558,11 +558,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,7 +905,7 @@
   <dimension ref="A1:I210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -918,10 +918,10 @@
       <c r="A1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -930,7 +930,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -941,7 +941,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -963,7 +963,7 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -974,7 +974,7 @@
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -985,21 +985,21 @@
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
update CIMAC IDs in template
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2B8F05-2EB1-6749-94C3-9445F585327E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96A8E29-0A3B-014C-9974-07B0C3C52138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7340" yWindow="4140" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -428,10 +428,10 @@
     <t>/local/path/to/rev.1.2.1.fastq.gz</t>
   </si>
   <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
+    <t>CTTTPP122.00</t>
+  </si>
+  <si>
+    <t>CTTTPP123.00</t>
   </si>
 </sst>
 </file>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -953,10 +953,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -964,7 +964,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
drop 'rqs' and 'rin' fields
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D53F0-2C01-C245-B93F-34EA0149AAC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5E0BD1-4E8F-A642-B74F-76891A62F120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7340" yWindow="4140" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,33 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>RNA quality score. (0-10)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>RNA integrity number. (0-10)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="72">
   <si>
     <t>LEGEND</t>
   </si>
@@ -902,19 +876,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I210"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="99" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -923,7 +897,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -934,7 +908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -945,7 +919,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -956,7 +930,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -967,7 +941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -978,7 +952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -989,7 +963,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>62</v>
       </c>
@@ -998,10 +972,8 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1021,16 +993,10 @@
         <v>32</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1050,13 +1016,10 @@
         <v>0.7</v>
       </c>
       <c r="G11">
-        <v>8</v>
-      </c>
-      <c r="I11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1076,31 +1039,25 @@
         <v>0.8</v>
       </c>
       <c r="G12">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>9</v>
-      </c>
-      <c r="I12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2078,7 +2035,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{1AE57A24-A028-7D4A-BB26-668046DD637A}">

</xml_diff>

<commit_message>
drop dv200 and quality_flag
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEE2B2-A988-0B4E-828D-4709229568E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8DE1F-70C5-004A-8C05-B00C38749FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="3220" windowWidth="21060" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8620" windowWidth="16700" windowHeight="8600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -159,38 +159,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The percentage of fragments &gt; 200 nucleotides.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Flag used for quality.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="64">
   <si>
     <t>LEGEND</t>
   </si>
@@ -288,18 +262,6 @@
     <t>Resulting yield (in ng) from library construction.</t>
   </si>
   <si>
-    <t>Dv200</t>
-  </si>
-  <si>
-    <t>The percentage of fragments &gt; 200 nucleotides.</t>
-  </si>
-  <si>
-    <t>Quality flag</t>
-  </si>
-  <si>
-    <t>Flag used for quality.</t>
-  </si>
-  <si>
     <t>DFCI</t>
   </si>
   <si>
@@ -375,25 +337,25 @@
     <t>#d</t>
   </si>
   <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>/local/path/to/fwd.1.1.1.fastq.gz,/local/path/to/fwd.1.1.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
-  </si>
-  <si>
     <t>/local/path/to/fwd.1.2.1.fastq.gz,/local/path/to/fwd.1.2.1_2.fastq.gz</t>
   </si>
   <si>
     <t>/local/path/to/rev.1.2.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.1.1.fastq.gz,/local/path/to/fwd.1.1.1_2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -848,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G210"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -860,94 +822,92 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
@@ -961,1053 +921,1035 @@
       <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
       </c>
       <c r="E11">
         <v>600</v>
       </c>
-      <c r="F11">
-        <v>0.7</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>650</v>
       </c>
-      <c r="F12">
-        <v>0.8</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2052,7 +1994,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2202,28 +2144,6 @@
       </c>
       <c r="D13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2262,69 +2182,69 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drop enrichment method, enrichment kit, paired end reads from preamble
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8DE1F-70C5-004A-8C05-B00C38749FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B55308-5FA3-A34E-9646-F43C7ED628FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8620" windowWidth="16700" windowHeight="8600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -62,50 +62,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Method used for enriching for mRNA.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Vendor for the bait set used for enrichment, e.g. Twist, Agilent, IDT.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Sequencer Model, e.g. HiSeq 2500, NextSeq, NovaSeq.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Indicates if the sequencing was performed paired or single ended.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -132,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="45">
   <si>
     <t>LEGEND</t>
   </si>
@@ -193,24 +154,6 @@
     <t>E.g. 'DFCI'</t>
   </si>
   <si>
-    <t>Enrichment method</t>
-  </si>
-  <si>
-    <t>Method used for enriching for mRNA.</t>
-  </si>
-  <si>
-    <t>E.g. 'PolyA capture'</t>
-  </si>
-  <si>
-    <t>Enrichment kit</t>
-  </si>
-  <si>
-    <t>Vendor for the bait set used for enrichment, e.g. Twist, Agilent, IDT.</t>
-  </si>
-  <si>
-    <t>E.g. 'Agilent'</t>
-  </si>
-  <si>
     <t>Sequencer platform</t>
   </si>
   <si>
@@ -220,15 +163,6 @@
     <t>E.g. 'Illumina - HiSeq 2500'</t>
   </si>
   <si>
-    <t>Paired end reads</t>
-  </si>
-  <si>
-    <t>Indicates if the sequencing was performed paired or single ended.</t>
-  </si>
-  <si>
-    <t>E.g. 'Paired'</t>
-  </si>
-  <si>
     <t>Section 'Samples' of tab 'TCR'</t>
   </si>
   <si>
@@ -274,30 +208,6 @@
     <t>MD Anderson</t>
   </si>
   <si>
-    <t>PolyA capture</t>
-  </si>
-  <si>
-    <t>Transcriptome capture</t>
-  </si>
-  <si>
-    <t>Ribo minus</t>
-  </si>
-  <si>
-    <t>Agilent</t>
-  </si>
-  <si>
-    <t>Twist</t>
-  </si>
-  <si>
-    <t>IDT</t>
-  </si>
-  <si>
-    <t>NEB</t>
-  </si>
-  <si>
-    <t>Illumina - TruSeq Stranded PolyA mRNA</t>
-  </si>
-  <si>
     <t>Illumina - HiSeq 2500</t>
   </si>
   <si>
@@ -313,12 +223,6 @@
     <t>Illumina - NovaSeq 6000</t>
   </si>
   <si>
-    <t>Paired</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
     <t>#t</t>
   </si>
   <si>
@@ -337,32 +241,32 @@
     <t>#d</t>
   </si>
   <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.1.1.fastq.gz,/local/path/to/fwd.1.1.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.1.fastq.gz,/local/path/to/fwd.1.2.1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
+  </si>
+  <si>
     <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.1.1.fastq.gz,/local/path/to/fwd.1.1.1_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.2.1.fastq.gz,/local/path/to/fwd.1.2.1_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +287,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -455,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -472,6 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,1140 +734,1107 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="6">
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="6">
+        <v>650</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11">
-        <v>600</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12">
-        <v>650</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Data Dictionary'!$B$2:$B$5</xm:f>
@@ -1964,27 +1843,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>'Data Dictionary'!$C$2:$C$4</xm:f>
+            <xm:f>'Data Dictionary'!$C$2:$C$6</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!$D$2:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!$E$2:$E$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1994,7 +1855,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2053,97 +1914,55 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>21</v>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2154,7 +1973,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:F6"/>
+  <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2163,88 +1982,49 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add batch_id & sample_sheet
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B55308-5FA3-A34E-9646-F43C7ED628FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213E169C-1D1E-F04B-808B-692F9B8DF829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,34 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TCRseq batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a user's computer.
+In .csv format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="51">
   <si>
     <t>LEGEND</t>
   </si>
@@ -163,6 +190,18 @@
     <t>E.g. 'Illumina - HiSeq 2500'</t>
   </si>
   <si>
+    <t>Batch id</t>
+  </si>
+  <si>
+    <t>TCRseq batch identification number.</t>
+  </si>
+  <si>
+    <t>Sample sheet</t>
+  </si>
+  <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
     <t>Section 'Samples' of tab 'TCR'</t>
   </si>
   <si>
@@ -260,13 +299,19 @@
   </si>
   <si>
     <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>sample_sheet.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,13 +332,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -366,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -383,7 +421,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -736,1099 +773,1121 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="6">
-        <v>600</v>
-      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="6">
-        <v>650</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11">
+        <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1855,7 +1914,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E10"/>
+  <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1914,55 +1973,77 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
+      <c r="E9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1992,39 +2073,39 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename fwd/rev fastq -> read 1/2 replicate
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E7E95C-0630-A440-B2F0-AEB9C58C9DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D51B26-276E-5448-ABC2-AD08EEB7971E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,12 +111,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A comma-separated list of paths to files on a user's computer.
-In .gz format</t>
+          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .gz format</t>
         </r>
       </text>
     </comment>
@@ -161,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="53">
   <si>
     <t>LEGEND</t>
   </si>
@@ -314,6 +323,12 @@
   </si>
   <si>
     <t>/local/path/to/fwd.1.2.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>Read 1 replicate x</t>
+  </si>
+  <si>
+    <t>Read 2 replicate x</t>
   </si>
 </sst>
 </file>
@@ -777,7 +792,7 @@
   <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -866,10 +881,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
add index replicate files
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D51B26-276E-5448-ABC2-AD08EEB7971E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F741F2E7-1C7F-A943-A09D-C3A2E75F5075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="17460" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,53 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{7CF4FD11-4519-E843-8F36-8CC235EBB76C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .gz format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{5FA88D75-8061-9A4D-94BF-E07692AEF394}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .gz format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="59">
   <si>
     <t>LEGEND</t>
   </si>
@@ -310,25 +356,43 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.2.1.fastq.gz</t>
-  </si>
-  <si>
     <t>Read 1 replicate x</t>
   </si>
   <si>
     <t>Read 2 replicate x</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read1_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read1_rx_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_rx_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>Index 1 replicate x</t>
+  </si>
+  <si>
+    <t>Index 2 replicate x</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_rx_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_rx_2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -789,19 +853,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="103" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -810,7 +874,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -821,7 +885,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -832,7 +896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -843,7 +907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -854,7 +918,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -865,15 +929,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -881,16 +947,22 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -898,53 +970,65 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="E10">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11">
         <v>650</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1917,7 +2001,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
regenerate final TCR template
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A6789-30FA-C04D-9FDD-1F4906DF00BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E63342-5BCD-4E4F-89B2-41770169D357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="17460" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{7CF4FD11-4519-E843-8F36-8CC235EBB76C}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{5FA88D75-8061-9A4D-94BF-E07692AEF394}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date when the TCR sequencing was run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="60">
   <si>
     <t>LEGEND</t>
   </si>
@@ -281,13 +294,28 @@
     <t>E.g. 'CTTTP01A1.00'</t>
   </si>
   <si>
-    <t>Forward fastq</t>
+    <t>Read 1 replicate x</t>
   </si>
   <si>
     <t>A comma-separated list of paths to files on a user's computer.</t>
   </si>
   <si>
-    <t>Reverse fastq</t>
+    <t>Read 2 replicate x</t>
+  </si>
+  <si>
+    <t>Index 1 replicate x</t>
+  </si>
+  <si>
+    <t>Index 2 replicate x</t>
+  </si>
+  <si>
+    <t>Sequencing run date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: date </t>
+  </si>
+  <si>
+    <t>Date when the TCR sequencing was run.</t>
   </si>
   <si>
     <t>Rna quantity</t>
@@ -356,46 +384,31 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>/local/path/to/read1_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_rx_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_rx_1.fastq.gz</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>Read 1 replicate x</t>
-  </si>
-  <si>
-    <t>Read 2 replicate x</t>
-  </si>
-  <si>
-    <t>/local/path/to/read2_rx_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/read1_rx_1.fastq.gz</t>
-  </si>
-  <si>
     <t>/local/path/to/read1_rx_2.fastq.gz</t>
   </si>
   <si>
     <t>/local/path/to/read2_rx_2.fastq.gz</t>
   </si>
   <si>
-    <t>Index 1 replicate x</t>
-  </si>
-  <si>
-    <t>Index 2 replicate x</t>
-  </si>
-  <si>
-    <t>/local/path/to/index1_rx_1.fastq.gz</t>
-  </si>
-  <si>
     <t>/local/path/to/index1_rx_2.fastq.gz</t>
   </si>
   <si>
-    <t>/local/path/to/index2_rx_1.fastq.gz</t>
-  </si>
-  <si>
     <t>/local/path/to/index2_rx_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>Sequencing run date</t>
   </si>
 </sst>
 </file>
@@ -859,83 +872,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="104" width="30.6640625" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -946,48 +959,48 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G10" s="6">
         <v>43811</v>
@@ -998,22 +1011,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G11" s="6">
         <v>43811</v>
@@ -1024,992 +1037,992 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2017,14 +2030,37 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B8:H8"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G10:G209" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>AND(ISNUMBER(G10:G209),LEFT(CELL("format",G10:G209),1)="D")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E12"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2150,10 +2186,43 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2183,39 +2252,39 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move sequencing_run_date to preamble
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E63342-5BCD-4E4F-89B2-41770169D357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23291D2-82A7-F548-A364-BDA99642C87B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="2800" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -88,12 +88,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Date when the TCR sequencing was run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Path to a file on a user's computer.
 In .csv format</t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -106,117 +119,68 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .gz format</t>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .gz format</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .gz format</t>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .gz format</t>
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .gz format</t>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .gz format</t>
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A comma-separated list of paths to files on a user's computer.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .gz format</t>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .gz format</t>
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date when the TCR sequencing was run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -229,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="60">
   <si>
     <t>LEGEND</t>
   </si>
@@ -273,6 +237,15 @@
     <t>TCRseq batch identification number.</t>
   </si>
   <si>
+    <t>Sequencing run date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: date </t>
+  </si>
+  <si>
+    <t>Date when the TCR sequencing was run.</t>
+  </si>
+  <si>
     <t>Sample sheet</t>
   </si>
   <si>
@@ -307,15 +280,6 @@
   </si>
   <si>
     <t>Index 2 replicate x</t>
-  </si>
-  <si>
-    <t>Sequencing run date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String: date </t>
-  </si>
-  <si>
-    <t>Date when the TCR sequencing was run.</t>
   </si>
   <si>
     <t>Rna quantity</t>
@@ -415,7 +379,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,12 +398,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -531,7 +489,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H209"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -882,7 +842,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -891,7 +851,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -902,7 +862,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -913,7 +873,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -924,7 +884,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -935,127 +895,123 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="6">
-        <v>43811</v>
-      </c>
-      <c r="H10">
+      <c r="G11">
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="6">
-        <v>43811</v>
-      </c>
-      <c r="H11">
+      <c r="G12">
         <v>650</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2022,39 +1978,21 @@
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:G9"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G10:G209" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>AND(ISNUMBER(G10:G209),LEFT(CELL("format",G10:G209),1)="D")</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2134,84 +2072,84 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
move index files to fastq_pair_or_bam.json
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23291D2-82A7-F548-A364-BDA99642C87B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C7BB98-7CE2-0142-AD80-233A0CDF1531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="2800" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,12 +354,6 @@
     <t>/local/path/to/read2_rx_1.fastq.gz</t>
   </si>
   <si>
-    <t>/local/path/to/index1_rx_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index2_rx_1.fastq.gz</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
@@ -369,10 +363,16 @@
     <t>/local/path/to/read2_rx_2.fastq.gz</t>
   </si>
   <si>
-    <t>/local/path/to/index1_rx_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index2_rx_2.fastq.gz</t>
+    <t>/local/path/to/index1_ix_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_ix_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_ix_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_ix_2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -486,11 +486,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +833,7 @@
   <dimension ref="A1:G210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,10 +846,10 @@
       <c r="A1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -902,7 +902,7 @@
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>43811</v>
       </c>
     </row>
@@ -918,14 +918,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -964,10 +964,10 @@
         <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>600</v>
@@ -978,13 +978,13 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Seperate TCR replicates, merge by replicate_no
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C7BB98-7CE2-0142-AD80-233A0CDF1531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72A06EB-73EB-EF4A-A6D8-5901BBD802F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="2800" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -128,8 +128,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A comma-separated list of paths to files on a user's computer.
-In .gz format</t>
+          <t>Replicate number.</t>
         </r>
       </text>
     </comment>
@@ -184,6 +183,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .gz format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>RNA quantity (in ng).</t>
         </r>
       </text>
@@ -193,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="62">
   <si>
     <t>LEGEND</t>
   </si>
@@ -267,27 +280,33 @@
     <t>E.g. 'CTTTP01A1.00'</t>
   </si>
   <si>
-    <t>Read 1 replicate x</t>
+    <t>Replicate no</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Replicate number.</t>
+  </si>
+  <si>
+    <t>Read 1</t>
   </si>
   <si>
     <t>A comma-separated list of paths to files on a user's computer.</t>
   </si>
   <si>
-    <t>Read 2 replicate x</t>
-  </si>
-  <si>
-    <t>Index 1 replicate x</t>
-  </si>
-  <si>
-    <t>Index 2 replicate x</t>
+    <t>Read 2</t>
+  </si>
+  <si>
+    <t>Index 1</t>
+  </si>
+  <si>
+    <t>Index 2</t>
   </si>
   <si>
     <t>Rna quantity</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>RNA quantity (in ng).</t>
   </si>
   <si>
@@ -327,59 +346,59 @@
     <t>#p</t>
   </si>
   <si>
-    <t>Samples</t>
-  </si>
-  <si>
     <t>#h</t>
   </si>
   <si>
     <t>#d</t>
   </si>
   <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/read1_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>/local/path/to/read1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_2.fastq.gz</t>
+  </si>
+  <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
     <t>XYZ</t>
   </si>
   <si>
-    <t>sample_sheet.csv</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>/local/path/to/read1_rx_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/read2_rx_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>/local/path/to/read1_rx_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/read2_rx_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index1_ix_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index2_ix_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index1_ix_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/index2_ix_2.fastq.gz</t>
+    <t>/local/path/to/sample_sheet.csv</t>
+  </si>
+  <si>
+    <t>Replicates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +417,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -830,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G210"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B9" sqref="B9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -842,62 +867,62 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
@@ -906,30 +931,31 @@
         <v>43811</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>20</v>
@@ -938,1067 +964,1099 @@
         <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11">
+      <c r="H11">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" t="s">
-        <v>58</v>
-      </c>
       <c r="F12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12">
+        <v>56</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12">
         <v>650</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>AND(ISNUMBER(C6),LEFT(CELL("format",C6),1)="D")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2113,54 +2171,65 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2190,39 +2259,39 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replicate_no (number) --> replicate_id (str)
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72A06EB-73EB-EF4A-A6D8-5901BBD802F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BDE905-CED6-A146-9306-5B45D75D4419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,7 +124,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="64">
   <si>
     <t>LEGEND</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>Replicates</t>
+  </si>
+  <si>
+    <t>Replicate id</t>
+  </si>
+  <si>
+    <t>1A</t>
   </si>
 </sst>
 </file>
@@ -858,7 +864,7 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -961,7 +967,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>27</v>
@@ -986,8 +992,8 @@
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -1012,8 +1018,8 @@
       <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C12">
-        <v>1</v>
+      <c r="C12" t="s">
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
make replicates an array
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1B4D3-864B-0F41-8E3D-6EF2B1338C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA171D31-51B8-F749-9FD2-898C7A9096EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1007,6 +1007,9 @@
       <c r="G11" t="s">
         <v>52</v>
       </c>
+      <c r="H11">
+        <v>600</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1029,6 +1032,9 @@
       </c>
       <c r="G12" t="s">
         <v>57</v>
+      </c>
+      <c r="H12">
+        <v>650</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add duplicate replicate for a sample
</commit_message>
<xml_diff>
--- a/template_examples/tcr_fastq_template.xlsx
+++ b/template_examples/tcr_fastq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA171D31-51B8-F749-9FD2-898C7A9096EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47987E2E-BB78-8D4D-89DB-C5D349548B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21960" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -97,12 +97,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .csv format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .csv format</t>
         </r>
       </text>
     </comment>
@@ -206,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="69">
   <si>
     <t>LEGEND</t>
   </si>
@@ -398,6 +407,34 @@
   </si>
   <si>
     <t>1A</t>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>/local/path/to/read1_3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/read2_3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index1_3.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/index2_3.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -863,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1040,6 +1077,27 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>